<commit_message>
Update economic factor impact by adjusting weightings for different sectors
Refactors impact weights in `export_impact_matrix.py` and `sentiment_engine.py` with sector-specific adjustments, and adds feedback file.

Replit-Commit-Author: Agent
Replit-Commit-Session-Id: 9f1fabd5-397e-4d58-99e6-ab2f6f3cc9f5
Replit-Commit-Screenshot-Url: https://storage.googleapis.com/screenshot-production-us-central1/56dde067-b2ce-481f-89f3-ffccd57ac11a/f2f91c4c-f85f-42e3-b1a4-07be23c4225d.jpg
</commit_message>
<xml_diff>
--- a/sector_impact_matrix.xlsx
+++ b/sector_impact_matrix.xlsx
@@ -710,7 +710,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
         <v>2</v>
@@ -759,7 +759,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
         <v>2</v>
@@ -906,7 +906,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
         <v>2</v>
@@ -915,16 +915,16 @@
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10" t="n">
         <v>2</v>
@@ -964,16 +964,16 @@
         <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" t="n">
         <v>3</v>
@@ -1053,10 +1053,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>3</v>
@@ -1065,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -1077,7 +1077,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
         <v>1</v>
@@ -1570,7 +1570,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C6" t="n">
         <v>2</v>
@@ -1619,7 +1619,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C7" t="n">
         <v>2</v>
@@ -1766,7 +1766,7 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C10" t="n">
         <v>2</v>
@@ -1775,16 +1775,16 @@
         <v>2</v>
       </c>
       <c r="E10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="F10" t="n">
         <v>2</v>
       </c>
       <c r="G10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H10" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I10" t="n">
         <v>2</v>
@@ -1824,16 +1824,16 @@
         <v>3</v>
       </c>
       <c r="E11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="F11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I11" t="n">
         <v>3</v>
@@ -1913,10 +1913,10 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D13" t="n">
         <v>3</v>
@@ -1925,7 +1925,7 @@
         <v>1</v>
       </c>
       <c r="F13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13" t="n">
         <v>1</v>
@@ -1937,7 +1937,7 @@
         <v>1</v>
       </c>
       <c r="J13" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K13" t="n">
         <v>1</v>

</xml_diff>